<commit_message>
cambiato il codice per ip dinamico per le github actions, manca lo yaml per i clan games e il file clan games è non funzionante
</commit_message>
<xml_diff>
--- a/prova.xlsx
+++ b/prova.xlsx
@@ -20,7 +20,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -42,12 +42,6 @@
       <b val="1"/>
       <color theme="0"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -152,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -202,11 +196,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -221,16 +211,416 @@
   </cellStyles>
   <dxfs count="70">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -299,418 +689,6 @@
       <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom"/>
-      <border>
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <name val="Aptos Narrow"/>
         <family val="2"/>
@@ -1019,6 +997,9 @@
       <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
       <font>
         <name val="Aptos Narrow"/>
         <family val="2"/>
@@ -1039,6 +1020,16 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom"/>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1061,6 +1052,14 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom"/>
+      <border outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1105,16 +1104,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom"/>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1137,14 +1126,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom"/>
-      <border outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1154,6 +1135,15 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
@@ -1235,7 +1225,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella2" displayName="Tabella2" ref="A1:AA51" headerRowCount="1" totalsRowShown="0" headerRowDxfId="0" dataDxfId="69" tableBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella2" displayName="Tabella2" ref="A1:AA51" headerRowCount="1" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="A1:AA51"/>
   <sortState ref="A2:AA51">
     <sortCondition ref="C2:C51"/>
@@ -1243,82 +1233,82 @@
     <sortCondition ref="A2:A51"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" name="NOME" dataDxfId="3"/>
-    <tableColumn id="2" name="DATA" dataDxfId="4"/>
-    <tableColumn id="3" name="MEDIA" dataDxfId="2"/>
-    <tableColumn id="4" name="TOTALE" dataDxfId="67"/>
-    <tableColumn id="5" name="ACHIEVMENT" dataDxfId="66"/>
-    <tableColumn id="27" name="22/10/2025" dataDxfId="1"/>
-    <tableColumn id="6" name="22/11/2025" dataDxfId="65"/>
-    <tableColumn id="7" name="22/12/2025" dataDxfId="64"/>
-    <tableColumn id="8" name="22/01/2026" dataDxfId="63"/>
-    <tableColumn id="9" name="22/02/2026" dataDxfId="62"/>
-    <tableColumn id="10" name="22/03/2026" dataDxfId="61"/>
-    <tableColumn id="11" name="22/04/2024" dataDxfId="60"/>
-    <tableColumn id="12" name="22/05/2026" dataDxfId="59"/>
-    <tableColumn id="13" name="22/06/2026" dataDxfId="58"/>
-    <tableColumn id="14" name="22/07/2026" dataDxfId="57"/>
-    <tableColumn id="15" name="Colonna10" dataDxfId="56"/>
-    <tableColumn id="16" name="Colonna11" dataDxfId="55"/>
-    <tableColumn id="17" name="Colonna12" dataDxfId="54"/>
-    <tableColumn id="18" name="Colonna13" dataDxfId="53"/>
-    <tableColumn id="19" name="Colonna14" dataDxfId="52"/>
-    <tableColumn id="20" name="Colonna15" dataDxfId="51"/>
-    <tableColumn id="21" name="Colonna16" dataDxfId="50"/>
-    <tableColumn id="22" name="Colonna17" dataDxfId="49"/>
-    <tableColumn id="23" name="Colonna18" dataDxfId="48"/>
-    <tableColumn id="24" name="Colonna19" dataDxfId="47"/>
-    <tableColumn id="25" name="Colonna20" dataDxfId="46"/>
-    <tableColumn id="26" name="Colonna21" dataDxfId="45"/>
+    <tableColumn id="1" name="NOME" dataDxfId="66"/>
+    <tableColumn id="2" name="DATA" dataDxfId="65"/>
+    <tableColumn id="3" name="MEDIA" dataDxfId="64"/>
+    <tableColumn id="4" name="TOTALE" dataDxfId="63"/>
+    <tableColumn id="5" name="ACHIEVMENT" dataDxfId="62"/>
+    <tableColumn id="27" name="22/10/2025" dataDxfId="61"/>
+    <tableColumn id="6" name="22/11/2025" dataDxfId="60"/>
+    <tableColumn id="7" name="22/12/2025" dataDxfId="59"/>
+    <tableColumn id="8" name="22/01/2026" dataDxfId="58"/>
+    <tableColumn id="9" name="22/02/2026" dataDxfId="57"/>
+    <tableColumn id="10" name="22/03/2026" dataDxfId="56"/>
+    <tableColumn id="11" name="22/04/2024" dataDxfId="55"/>
+    <tableColumn id="12" name="22/05/2026" dataDxfId="54"/>
+    <tableColumn id="13" name="22/06/2026" dataDxfId="53"/>
+    <tableColumn id="14" name="22/07/2026" dataDxfId="52"/>
+    <tableColumn id="15" name="Colonna10" dataDxfId="51"/>
+    <tableColumn id="16" name="Colonna11" dataDxfId="50"/>
+    <tableColumn id="17" name="Colonna12" dataDxfId="49"/>
+    <tableColumn id="18" name="Colonna13" dataDxfId="48"/>
+    <tableColumn id="19" name="Colonna14" dataDxfId="47"/>
+    <tableColumn id="20" name="Colonna15" dataDxfId="46"/>
+    <tableColumn id="21" name="Colonna16" dataDxfId="45"/>
+    <tableColumn id="22" name="Colonna17" dataDxfId="44"/>
+    <tableColumn id="23" name="Colonna18" dataDxfId="43"/>
+    <tableColumn id="24" name="Colonna19" dataDxfId="42"/>
+    <tableColumn id="25" name="Colonna20" dataDxfId="41"/>
+    <tableColumn id="26" name="Colonna21" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabella1" displayName="Tabella1" ref="A1:AK51" headerRowCount="1" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabella1" displayName="Tabella1" ref="A1:AK51" headerRowCount="1" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:AK51"/>
   <sortState ref="A2:AK51">
     <sortCondition ref="C1:C51"/>
   </sortState>
   <tableColumns count="37">
-    <tableColumn id="1" name="NOME" dataDxfId="42"/>
-    <tableColumn id="2" name="DATA" dataDxfId="41"/>
-    <tableColumn id="3" name="MEDIA" dataDxfId="40"/>
-    <tableColumn id="4" name="23/11/2025" dataDxfId="39"/>
-    <tableColumn id="5" name="30/11/2025" dataDxfId="38"/>
-    <tableColumn id="6" name="07/12/2025" dataDxfId="37"/>
-    <tableColumn id="7" name="14/12/2025" dataDxfId="36"/>
-    <tableColumn id="8" name="19/12/2025" dataDxfId="35"/>
-    <tableColumn id="9" name="Colonna1" dataDxfId="34"/>
-    <tableColumn id="10" name="Colonna5" dataDxfId="33"/>
-    <tableColumn id="11" name="Colonna6" dataDxfId="32"/>
-    <tableColumn id="12" name="Colonna7" dataDxfId="31"/>
-    <tableColumn id="13" name="Colonna8" dataDxfId="30"/>
-    <tableColumn id="14" name="Colonna9" dataDxfId="29"/>
-    <tableColumn id="15" name="Colonna10" dataDxfId="28"/>
-    <tableColumn id="16" name="Colonna11" dataDxfId="27"/>
-    <tableColumn id="17" name="Colonna12" dataDxfId="26"/>
-    <tableColumn id="18" name="Colonna13" dataDxfId="25"/>
-    <tableColumn id="19" name="Colonna14" dataDxfId="24"/>
-    <tableColumn id="20" name="Colonna15" dataDxfId="23"/>
-    <tableColumn id="21" name="Colonna16" dataDxfId="22"/>
-    <tableColumn id="22" name="Colonna17" dataDxfId="21"/>
-    <tableColumn id="23" name="Colonna18" dataDxfId="20"/>
-    <tableColumn id="24" name="Colonna19" dataDxfId="19"/>
-    <tableColumn id="25" name="Colonna20" dataDxfId="18"/>
-    <tableColumn id="26" name="Colonna21" dataDxfId="17"/>
-    <tableColumn id="27" name="Colonna22" dataDxfId="16"/>
-    <tableColumn id="28" name="Colonna23" dataDxfId="15"/>
-    <tableColumn id="29" name="Colonna24" dataDxfId="14"/>
-    <tableColumn id="30" name="Colonna25" dataDxfId="13"/>
-    <tableColumn id="31" name="Colonna26" dataDxfId="12"/>
-    <tableColumn id="32" name="Colonna27" dataDxfId="11"/>
-    <tableColumn id="33" name="Colonna28" dataDxfId="10"/>
-    <tableColumn id="34" name="Colonna29" dataDxfId="9"/>
-    <tableColumn id="35" name="Colonna30" dataDxfId="8"/>
-    <tableColumn id="36" name="Colonna31" dataDxfId="7"/>
-    <tableColumn id="37" name="Colonna32" dataDxfId="6"/>
+    <tableColumn id="1" name="NOME" dataDxfId="37"/>
+    <tableColumn id="2" name="DATA" dataDxfId="36"/>
+    <tableColumn id="3" name="MEDIA" dataDxfId="35"/>
+    <tableColumn id="4" name="23/11/2025" dataDxfId="34"/>
+    <tableColumn id="5" name="30/11/2025" dataDxfId="33"/>
+    <tableColumn id="6" name="07/12/2025" dataDxfId="32"/>
+    <tableColumn id="7" name="14/12/2025" dataDxfId="31"/>
+    <tableColumn id="8" name="19/12/2025" dataDxfId="30"/>
+    <tableColumn id="9" name="Colonna1" dataDxfId="29"/>
+    <tableColumn id="10" name="Colonna5" dataDxfId="28"/>
+    <tableColumn id="11" name="Colonna6" dataDxfId="27"/>
+    <tableColumn id="12" name="Colonna7" dataDxfId="26"/>
+    <tableColumn id="13" name="Colonna8" dataDxfId="25"/>
+    <tableColumn id="14" name="Colonna9" dataDxfId="24"/>
+    <tableColumn id="15" name="Colonna10" dataDxfId="23"/>
+    <tableColumn id="16" name="Colonna11" dataDxfId="22"/>
+    <tableColumn id="17" name="Colonna12" dataDxfId="21"/>
+    <tableColumn id="18" name="Colonna13" dataDxfId="20"/>
+    <tableColumn id="19" name="Colonna14" dataDxfId="19"/>
+    <tableColumn id="20" name="Colonna15" dataDxfId="18"/>
+    <tableColumn id="21" name="Colonna16" dataDxfId="17"/>
+    <tableColumn id="22" name="Colonna17" dataDxfId="16"/>
+    <tableColumn id="23" name="Colonna18" dataDxfId="15"/>
+    <tableColumn id="24" name="Colonna19" dataDxfId="14"/>
+    <tableColumn id="25" name="Colonna20" dataDxfId="13"/>
+    <tableColumn id="26" name="Colonna21" dataDxfId="12"/>
+    <tableColumn id="27" name="Colonna22" dataDxfId="11"/>
+    <tableColumn id="28" name="Colonna23" dataDxfId="10"/>
+    <tableColumn id="29" name="Colonna24" dataDxfId="9"/>
+    <tableColumn id="30" name="Colonna25" dataDxfId="8"/>
+    <tableColumn id="31" name="Colonna26" dataDxfId="7"/>
+    <tableColumn id="32" name="Colonna27" dataDxfId="6"/>
+    <tableColumn id="33" name="Colonna28" dataDxfId="5"/>
+    <tableColumn id="34" name="Colonna29" dataDxfId="4"/>
+    <tableColumn id="35" name="Colonna30" dataDxfId="3"/>
+    <tableColumn id="36" name="Colonna31" dataDxfId="2"/>
+    <tableColumn id="37" name="Colonna32" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1331,7 +1321,7 @@
     <sortCondition ref="B1:B51"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" name="NOMEE" dataDxfId="5"/>
+    <tableColumn id="1" name="NOMEE" dataDxfId="0"/>
     <tableColumn id="2" name="ASCIA"/>
     <tableColumn id="3" name="Colonna2"/>
     <tableColumn id="4" name="Colonna3"/>
@@ -1676,30 +1666,30 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA50"/>
+  <dimension ref="A1:AA49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14.28515625" customWidth="1" style="17" min="1" max="1"/>
-    <col width="16.28515625" customWidth="1" style="17" min="2" max="2"/>
-    <col width="13" customWidth="1" style="17" min="3" max="3"/>
-    <col width="9.85546875" customWidth="1" style="17" min="4" max="4"/>
-    <col width="13.140625" customWidth="1" style="17" min="5" max="6"/>
-    <col width="8.7109375" customWidth="1" style="17" min="7" max="7"/>
-    <col width="9.42578125" customWidth="1" style="17" min="8" max="8"/>
-    <col width="13.85546875" customWidth="1" style="17" min="9" max="9"/>
-    <col width="14.28515625" customWidth="1" style="17" min="10" max="10"/>
-    <col width="11.7109375" customWidth="1" style="17" min="11" max="15"/>
-    <col width="12.7109375" customWidth="1" style="17" min="16" max="23"/>
-    <col width="12.5703125" customWidth="1" style="17" min="24" max="27"/>
+    <col width="14.28515625" customWidth="1" min="1" max="1"/>
+    <col width="16.28515625" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="9.85546875" customWidth="1" min="4" max="4"/>
+    <col width="13.140625" customWidth="1" min="5" max="6"/>
+    <col width="8.7109375" customWidth="1" min="7" max="7"/>
+    <col width="9.42578125" customWidth="1" min="8" max="8"/>
+    <col width="13.85546875" customWidth="1" min="9" max="9"/>
+    <col width="14.28515625" customWidth="1" min="10" max="10"/>
+    <col width="11.7109375" customWidth="1" min="11" max="15"/>
+    <col width="12.7109375" customWidth="1" min="16" max="23"/>
+    <col width="12.5703125" customWidth="1" min="24" max="27"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="17" thickBot="1">
-      <c r="A1" s="19" t="inlineStr">
+    <row r="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>NOME</t>
         </is>
@@ -1709,17 +1699,17 @@
           <t>DATA</t>
         </is>
       </c>
-      <c r="C1" s="20" t="inlineStr">
+      <c r="C1" s="18" t="inlineStr">
         <is>
           <t>MEDIA</t>
         </is>
       </c>
-      <c r="D1" s="19" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>TOTALE</t>
         </is>
       </c>
-      <c r="E1" s="21" t="inlineStr">
+      <c r="E1" s="19" t="inlineStr">
         <is>
           <t>ACHIEVMENT</t>
         </is>
@@ -1841,7 +1831,7 @@
           <t>Chabby</t>
         </is>
       </c>
-      <c r="B2" s="18" t="inlineStr">
+      <c r="B2" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -1861,7 +1851,9 @@
       <c r="G2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="n"/>
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I2" s="1" t="n"/>
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
@@ -1884,7 +1876,7 @@
           <t>D 011</t>
         </is>
       </c>
-      <c r="B3" s="18" t="inlineStr">
+      <c r="B3" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -1904,7 +1896,9 @@
       <c r="G3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="n"/>
+      <c r="H3" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I3" s="1" t="n"/>
       <c r="J3" s="1" t="n"/>
       <c r="K3" s="1" t="n"/>
@@ -1927,7 +1921,7 @@
           <t>gionny</t>
         </is>
       </c>
-      <c r="B4" s="18" t="inlineStr">
+      <c r="B4" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -1947,7 +1941,9 @@
       <c r="G4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="1" t="n"/>
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I4" s="1" t="n"/>
       <c r="J4" s="1" t="n"/>
       <c r="K4" s="1" t="n"/>
@@ -1970,7 +1966,7 @@
           <t>zombra</t>
         </is>
       </c>
-      <c r="B5" s="18" t="inlineStr">
+      <c r="B5" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -1990,7 +1986,9 @@
       <c r="G5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="1" t="n"/>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>
       <c r="K5" s="1" t="n"/>
@@ -2013,7 +2011,7 @@
           <t>sono io lakaka</t>
         </is>
       </c>
-      <c r="B6" s="18" t="inlineStr">
+      <c r="B6" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2033,7 +2031,9 @@
       <c r="G6" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="H6" s="1" t="n"/>
+      <c r="H6" s="1" t="n">
+        <v>450</v>
+      </c>
       <c r="I6" s="1" t="n"/>
       <c r="J6" s="1" t="n"/>
       <c r="K6" s="1" t="n"/>
@@ -2056,7 +2056,7 @@
           <t>lord pucci</t>
         </is>
       </c>
-      <c r="B7" s="18" t="inlineStr">
+      <c r="B7" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2076,7 +2076,9 @@
       <c r="G7" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="H7" s="1" t="n"/>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I7" s="1" t="n"/>
       <c r="J7" s="1" t="n"/>
       <c r="K7" s="1" t="n"/>
@@ -2099,7 +2101,7 @@
           <t>Luxor</t>
         </is>
       </c>
-      <c r="B8" s="18" t="inlineStr">
+      <c r="B8" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2121,7 +2123,9 @@
       <c r="G8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="1" t="n"/>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I8" s="1" t="n"/>
       <c r="J8" s="1" t="n"/>
       <c r="K8" s="1" t="n"/>
@@ -2144,13 +2148,13 @@
           <t>giosan</t>
         </is>
       </c>
-      <c r="B9" s="18" t="inlineStr">
+      <c r="B9" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
       <c r="C9" s="2">
-        <f>AVERAGE(F9:AB9)</f>
+        <f>ROUND(AVERAGE(F9:AB9),1)</f>
         <v/>
       </c>
       <c r="D9" s="3">
@@ -2166,7 +2170,9 @@
       <c r="G9" s="1" t="n">
         <v>2450</v>
       </c>
-      <c r="H9" s="1" t="n"/>
+      <c r="H9" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I9" s="1" t="n"/>
       <c r="J9" s="1" t="n"/>
       <c r="K9" s="1" t="n"/>
@@ -2189,7 +2195,7 @@
           <t>dux104</t>
         </is>
       </c>
-      <c r="B10" s="18" t="inlineStr">
+      <c r="B10" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2211,7 +2217,9 @@
       <c r="G10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="1" t="n"/>
+      <c r="H10" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I10" s="1" t="n"/>
       <c r="J10" s="1" t="n"/>
       <c r="K10" s="1" t="n"/>
@@ -2234,7 +2242,7 @@
           <t>maikol_lix</t>
         </is>
       </c>
-      <c r="B11" s="18" t="inlineStr">
+      <c r="B11" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2256,7 +2264,9 @@
       <c r="G11" s="1" t="n">
         <v>2100</v>
       </c>
-      <c r="H11" s="1" t="n"/>
+      <c r="H11" s="1" t="n">
+        <v>1500</v>
+      </c>
       <c r="I11" s="1" t="n"/>
       <c r="J11" s="1" t="n"/>
       <c r="K11" s="1" t="n"/>
@@ -2279,7 +2289,7 @@
           <t>ajejebrazorf</t>
         </is>
       </c>
-      <c r="B12" s="18" t="inlineStr">
+      <c r="B12" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2299,7 +2309,9 @@
       <c r="G12" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H12" s="1" t="n"/>
+      <c r="H12" s="1" t="n">
+        <v>3250</v>
+      </c>
       <c r="I12" s="1" t="n"/>
       <c r="J12" s="1" t="n"/>
       <c r="K12" s="1" t="n"/>
@@ -2322,7 +2334,7 @@
           <t>HikariNoRob</t>
         </is>
       </c>
-      <c r="B13" s="18" t="inlineStr">
+      <c r="B13" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2342,7 +2354,9 @@
       <c r="G13" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H13" s="1" t="n"/>
+      <c r="H13" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I13" s="1" t="n"/>
       <c r="J13" s="1" t="n"/>
       <c r="K13" s="1" t="n"/>
@@ -2365,7 +2379,7 @@
           <t>kakko garau</t>
         </is>
       </c>
-      <c r="B14" s="18" t="inlineStr">
+      <c r="B14" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2385,7 +2399,9 @@
       <c r="G14" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H14" s="1" t="n"/>
+      <c r="H14" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I14" s="1" t="n"/>
       <c r="J14" s="1" t="n"/>
       <c r="K14" s="1" t="n"/>
@@ -2408,7 +2424,7 @@
           <t>leo</t>
         </is>
       </c>
-      <c r="B15" s="18" t="inlineStr">
+      <c r="B15" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2428,7 +2444,9 @@
       <c r="G15" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H15" s="1" t="n"/>
+      <c r="H15" s="1" t="n">
+        <v>5050</v>
+      </c>
       <c r="I15" s="1" t="n"/>
       <c r="J15" s="1" t="n"/>
       <c r="K15" s="1" t="n"/>
@@ -2451,7 +2469,7 @@
           <t>luigi01</t>
         </is>
       </c>
-      <c r="B16" s="18" t="inlineStr">
+      <c r="B16" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2471,7 +2489,9 @@
       <c r="G16" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H16" s="1" t="n"/>
+      <c r="H16" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I16" s="1" t="n"/>
       <c r="J16" s="1" t="n"/>
       <c r="K16" s="1" t="n"/>
@@ -2494,7 +2514,7 @@
           <t>Roberta</t>
         </is>
       </c>
-      <c r="B17" s="18" t="inlineStr">
+      <c r="B17" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2514,7 +2534,9 @@
       <c r="G17" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H17" s="1" t="n"/>
+      <c r="H17" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I17" s="1" t="n"/>
       <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
@@ -2537,7 +2559,7 @@
           <t>sidcu js</t>
         </is>
       </c>
-      <c r="B18" s="18" t="inlineStr">
+      <c r="B18" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2557,7 +2579,9 @@
       <c r="G18" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H18" s="1" t="n"/>
+      <c r="H18" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I18" s="1" t="n"/>
       <c r="J18" s="1" t="n"/>
       <c r="K18" s="1" t="n"/>
@@ -2580,7 +2604,7 @@
           <t>Simone</t>
         </is>
       </c>
-      <c r="B19" s="18" t="inlineStr">
+      <c r="B19" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2600,7 +2624,9 @@
       <c r="G19" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H19" s="1" t="n"/>
+      <c r="H19" s="1" t="n">
+        <v>400</v>
+      </c>
       <c r="I19" s="1" t="n"/>
       <c r="J19" s="1" t="n"/>
       <c r="K19" s="1" t="n"/>
@@ -2623,7 +2649,7 @@
           <t>Brazo</t>
         </is>
       </c>
-      <c r="B20" s="18" t="inlineStr">
+      <c r="B20" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2645,7 +2671,9 @@
       <c r="G20" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H20" s="1" t="n"/>
+      <c r="H20" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I20" s="1" t="n"/>
       <c r="J20" s="1" t="n"/>
       <c r="K20" s="1" t="n"/>
@@ -2668,7 +2696,7 @@
           <t>buff x-bow</t>
         </is>
       </c>
-      <c r="B21" s="18" t="inlineStr">
+      <c r="B21" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2690,7 +2718,9 @@
       <c r="G21" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H21" s="1" t="n"/>
+      <c r="H21" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I21" s="1" t="n"/>
       <c r="J21" s="1" t="n"/>
       <c r="K21" s="1" t="n"/>
@@ -2713,7 +2743,7 @@
           <t>Cleopatra</t>
         </is>
       </c>
-      <c r="B22" s="18" t="inlineStr">
+      <c r="B22" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2735,7 +2765,9 @@
       <c r="G22" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H22" s="1" t="n"/>
+      <c r="H22" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I22" s="1" t="n"/>
       <c r="J22" s="1" t="n"/>
       <c r="K22" s="1" t="n"/>
@@ -2758,7 +2790,7 @@
           <t>Floky23</t>
         </is>
       </c>
-      <c r="B23" s="18" t="inlineStr">
+      <c r="B23" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2780,7 +2812,9 @@
       <c r="G23" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H23" s="1" t="n"/>
+      <c r="H23" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I23" s="1" t="n"/>
       <c r="J23" s="1" t="n"/>
       <c r="K23" s="1" t="n"/>
@@ -2803,7 +2837,7 @@
           <t>haha</t>
         </is>
       </c>
-      <c r="B24" s="18" t="inlineStr">
+      <c r="B24" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2825,7 +2859,9 @@
       <c r="G24" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H24" s="1" t="n"/>
+      <c r="H24" s="1" t="n">
+        <v>450</v>
+      </c>
       <c r="I24" s="1" t="n"/>
       <c r="J24" s="1" t="n"/>
       <c r="K24" s="1" t="n"/>
@@ -2848,7 +2884,7 @@
           <t>RobbyCV</t>
         </is>
       </c>
-      <c r="B25" s="18" t="inlineStr">
+      <c r="B25" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2870,7 +2906,9 @@
       <c r="G25" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H25" s="1" t="n"/>
+      <c r="H25" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I25" s="1" t="n"/>
       <c r="J25" s="1" t="n"/>
       <c r="K25" s="1" t="n"/>
@@ -2893,7 +2931,7 @@
           <t>serra008</t>
         </is>
       </c>
-      <c r="B26" s="18" t="inlineStr">
+      <c r="B26" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2915,7 +2953,9 @@
       <c r="G26" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H26" s="1" t="n"/>
+      <c r="H26" s="1" t="n">
+        <v>2100</v>
+      </c>
       <c r="I26" s="1" t="n"/>
       <c r="J26" s="1" t="n"/>
       <c r="K26" s="1" t="n"/>
@@ -2938,7 +2978,7 @@
           <t>Stentaaa</t>
         </is>
       </c>
-      <c r="B27" s="18" t="inlineStr">
+      <c r="B27" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -2960,7 +3000,9 @@
       <c r="G27" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H27" s="1" t="n"/>
+      <c r="H27" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I27" s="1" t="n"/>
       <c r="J27" s="1" t="n"/>
       <c r="K27" s="1" t="n"/>
@@ -2983,7 +3025,7 @@
           <t>th4nos</t>
         </is>
       </c>
-      <c r="B28" s="18" t="inlineStr">
+      <c r="B28" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3005,7 +3047,9 @@
       <c r="G28" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="H28" s="1" t="n"/>
+      <c r="H28" s="1" t="n">
+        <v>950</v>
+      </c>
       <c r="I28" s="1" t="n"/>
       <c r="J28" s="1" t="n"/>
       <c r="K28" s="1" t="n"/>
@@ -3028,7 +3072,7 @@
           <t>BigMc23</t>
         </is>
       </c>
-      <c r="B29" s="18" t="inlineStr">
+      <c r="B29" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3046,7 +3090,9 @@
       </c>
       <c r="F29" s="1" t="n"/>
       <c r="G29" s="1" t="n"/>
-      <c r="H29" s="1" t="n"/>
+      <c r="H29" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I29" s="1" t="n"/>
       <c r="J29" s="1" t="n"/>
       <c r="K29" s="1" t="n"/>
@@ -3069,7 +3115,7 @@
           <t>dado</t>
         </is>
       </c>
-      <c r="B30" s="18" t="inlineStr">
+      <c r="B30" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3087,7 +3133,9 @@
       </c>
       <c r="F30" s="1" t="n"/>
       <c r="G30" s="1" t="n"/>
-      <c r="H30" s="1" t="n"/>
+      <c r="H30" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I30" s="1" t="n"/>
       <c r="J30" s="1" t="n"/>
       <c r="K30" s="1" t="n"/>
@@ -3110,7 +3158,7 @@
           <t>piegian99</t>
         </is>
       </c>
-      <c r="B31" s="18" t="inlineStr">
+      <c r="B31" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3128,7 +3176,9 @@
       </c>
       <c r="F31" s="1" t="n"/>
       <c r="G31" s="1" t="n"/>
-      <c r="H31" s="1" t="n"/>
+      <c r="H31" s="1" t="n">
+        <v>10000</v>
+      </c>
       <c r="I31" s="1" t="n"/>
       <c r="J31" s="1" t="n"/>
       <c r="K31" s="1" t="n"/>
@@ -3151,7 +3201,7 @@
           <t>EdoDodo</t>
         </is>
       </c>
-      <c r="B32" s="18" t="inlineStr">
+      <c r="B32" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3169,7 +3219,9 @@
       </c>
       <c r="F32" s="1" t="n"/>
       <c r="G32" s="1" t="n"/>
-      <c r="H32" s="1" t="n"/>
+      <c r="H32" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I32" s="1" t="n"/>
       <c r="J32" s="1" t="n"/>
       <c r="K32" s="1" t="n"/>
@@ -3192,7 +3244,7 @@
           <t>CARFI</t>
         </is>
       </c>
-      <c r="B33" s="18" t="inlineStr">
+      <c r="B33" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3210,7 +3262,9 @@
       </c>
       <c r="F33" s="1" t="n"/>
       <c r="G33" s="1" t="n"/>
-      <c r="H33" s="1" t="n"/>
+      <c r="H33" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I33" s="1" t="n"/>
       <c r="J33" s="1" t="n"/>
       <c r="K33" s="1" t="n"/>
@@ -3233,7 +3287,7 @@
           <t>pigiamone99</t>
         </is>
       </c>
-      <c r="B34" s="18" t="inlineStr">
+      <c r="B34" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3251,7 +3305,9 @@
       </c>
       <c r="F34" s="1" t="n"/>
       <c r="G34" s="1" t="n"/>
-      <c r="H34" s="1" t="n"/>
+      <c r="H34" s="1" t="n">
+        <v>3850</v>
+      </c>
       <c r="I34" s="1" t="n"/>
       <c r="J34" s="1" t="n"/>
       <c r="K34" s="1" t="n"/>
@@ -3274,7 +3330,7 @@
           <t>Rosario</t>
         </is>
       </c>
-      <c r="B35" s="18" t="inlineStr">
+      <c r="B35" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3292,7 +3348,9 @@
       </c>
       <c r="F35" s="1" t="n"/>
       <c r="G35" s="1" t="n"/>
-      <c r="H35" s="1" t="n"/>
+      <c r="H35" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I35" s="1" t="n"/>
       <c r="J35" s="1" t="n"/>
       <c r="K35" s="1" t="n"/>
@@ -3315,7 +3373,7 @@
           <t>LELE11GAM3R</t>
         </is>
       </c>
-      <c r="B36" s="18" t="inlineStr">
+      <c r="B36" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3333,7 +3391,9 @@
       </c>
       <c r="F36" s="1" t="n"/>
       <c r="G36" s="1" t="n"/>
-      <c r="H36" s="1" t="n"/>
+      <c r="H36" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I36" s="1" t="n"/>
       <c r="J36" s="1" t="n"/>
       <c r="K36" s="1" t="n"/>
@@ -3356,7 +3416,7 @@
           <t>ER DANDI 1927</t>
         </is>
       </c>
-      <c r="B37" s="18" t="inlineStr">
+      <c r="B37" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3374,7 +3434,9 @@
       </c>
       <c r="F37" s="1" t="n"/>
       <c r="G37" s="1" t="n"/>
-      <c r="H37" s="1" t="n"/>
+      <c r="H37" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I37" s="1" t="n"/>
       <c r="J37" s="1" t="n"/>
       <c r="K37" s="1" t="n"/>
@@ -3397,7 +3459,7 @@
           <t>SubOhm</t>
         </is>
       </c>
-      <c r="B38" s="18" t="inlineStr">
+      <c r="B38" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3415,7 +3477,9 @@
       </c>
       <c r="F38" s="1" t="n"/>
       <c r="G38" s="1" t="n"/>
-      <c r="H38" s="1" t="n"/>
+      <c r="H38" s="1" t="n">
+        <v>600</v>
+      </c>
       <c r="I38" s="1" t="n"/>
       <c r="J38" s="1" t="n"/>
       <c r="K38" s="1" t="n"/>
@@ -3438,7 +3502,7 @@
           <t>Luigi</t>
         </is>
       </c>
-      <c r="B39" s="18" t="inlineStr">
+      <c r="B39" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3456,7 +3520,9 @@
       </c>
       <c r="F39" s="1" t="n"/>
       <c r="G39" s="1" t="n"/>
-      <c r="H39" s="1" t="n"/>
+      <c r="H39" s="1" t="n">
+        <v>400</v>
+      </c>
       <c r="I39" s="1" t="n"/>
       <c r="J39" s="1" t="n"/>
       <c r="K39" s="1" t="n"/>
@@ -3479,7 +3545,7 @@
           <t>Valh</t>
         </is>
       </c>
-      <c r="B40" s="18" t="inlineStr">
+      <c r="B40" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3497,7 +3563,9 @@
       </c>
       <c r="F40" s="1" t="n"/>
       <c r="G40" s="1" t="n"/>
-      <c r="H40" s="1" t="n"/>
+      <c r="H40" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I40" s="1" t="n"/>
       <c r="J40" s="1" t="n"/>
       <c r="K40" s="1" t="n"/>
@@ -3520,7 +3588,7 @@
           <t>xbladze</t>
         </is>
       </c>
-      <c r="B41" s="18" t="inlineStr">
+      <c r="B41" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3538,7 +3606,9 @@
       </c>
       <c r="F41" s="1" t="n"/>
       <c r="G41" s="1" t="n"/>
-      <c r="H41" s="1" t="n"/>
+      <c r="H41" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I41" s="1" t="n"/>
       <c r="J41" s="1" t="n"/>
       <c r="K41" s="1" t="n"/>
@@ -3561,7 +3631,7 @@
           <t>tustrunz</t>
         </is>
       </c>
-      <c r="B42" s="18" t="inlineStr">
+      <c r="B42" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3579,7 +3649,9 @@
       </c>
       <c r="F42" s="1" t="n"/>
       <c r="G42" s="1" t="n"/>
-      <c r="H42" s="1" t="n"/>
+      <c r="H42" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I42" s="1" t="n"/>
       <c r="J42" s="1" t="n"/>
       <c r="K42" s="1" t="n"/>
@@ -3599,10 +3671,10 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>hh</t>
-        </is>
-      </c>
-      <c r="B43" s="18" t="inlineStr">
+          <t>marcojk007</t>
+        </is>
+      </c>
+      <c r="B43" s="17" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
@@ -3616,11 +3688,13 @@
         <v/>
       </c>
       <c r="E43" s="5" t="n">
-        <v>1450</v>
+        <v>70660</v>
       </c>
       <c r="F43" s="1" t="n"/>
       <c r="G43" s="1" t="n"/>
-      <c r="H43" s="1" t="n"/>
+      <c r="H43" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I43" s="1" t="n"/>
       <c r="J43" s="1" t="n"/>
       <c r="K43" s="1" t="n"/>
@@ -3640,12 +3714,12 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>marcojk007</t>
-        </is>
-      </c>
-      <c r="B44" s="18" t="inlineStr">
-        <is>
-          <t>15/12/2025</t>
+          <t>shark</t>
+        </is>
+      </c>
+      <c r="B44" s="17" t="inlineStr">
+        <is>
+          <t>19/12/2025</t>
         </is>
       </c>
       <c r="C44" s="2">
@@ -3657,11 +3731,13 @@
         <v/>
       </c>
       <c r="E44" s="5" t="n">
-        <v>70660</v>
+        <v>505</v>
       </c>
       <c r="F44" s="1" t="n"/>
       <c r="G44" s="1" t="n"/>
-      <c r="H44" s="1" t="n"/>
+      <c r="H44" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I44" s="1" t="n"/>
       <c r="J44" s="1" t="n"/>
       <c r="K44" s="1" t="n"/>
@@ -3681,10 +3757,10 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>shark</t>
-        </is>
-      </c>
-      <c r="B45" s="18" t="inlineStr">
+          <t>king</t>
+        </is>
+      </c>
+      <c r="B45" s="17" t="inlineStr">
         <is>
           <t>19/12/2025</t>
         </is>
@@ -3698,11 +3774,13 @@
         <v/>
       </c>
       <c r="E45" s="5" t="n">
-        <v>505</v>
+        <v>39890</v>
       </c>
       <c r="F45" s="1" t="n"/>
       <c r="G45" s="1" t="n"/>
-      <c r="H45" s="1" t="n"/>
+      <c r="H45" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I45" s="1" t="n"/>
       <c r="J45" s="1" t="n"/>
       <c r="K45" s="1" t="n"/>
@@ -3722,10 +3800,10 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>king</t>
-        </is>
-      </c>
-      <c r="B46" s="18" t="inlineStr">
+          <t>gh</t>
+        </is>
+      </c>
+      <c r="B46" s="17" t="inlineStr">
         <is>
           <t>19/12/2025</t>
         </is>
@@ -3739,11 +3817,13 @@
         <v/>
       </c>
       <c r="E46" s="5" t="n">
-        <v>39890</v>
+        <v>7100</v>
       </c>
       <c r="F46" s="1" t="n"/>
       <c r="G46" s="1" t="n"/>
-      <c r="H46" s="1" t="n"/>
+      <c r="H46" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I46" s="1" t="n"/>
       <c r="J46" s="1" t="n"/>
       <c r="K46" s="1" t="n"/>
@@ -3763,10 +3843,10 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>gh</t>
-        </is>
-      </c>
-      <c r="B47" s="18" t="inlineStr">
+          <t>Matty7_</t>
+        </is>
+      </c>
+      <c r="B47" s="17" t="inlineStr">
         <is>
           <t>19/12/2025</t>
         </is>
@@ -3780,11 +3860,13 @@
         <v/>
       </c>
       <c r="E47" s="5" t="n">
-        <v>7100</v>
+        <v>34720</v>
       </c>
       <c r="F47" s="1" t="n"/>
       <c r="G47" s="1" t="n"/>
-      <c r="H47" s="1" t="n"/>
+      <c r="H47" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I47" s="1" t="n"/>
       <c r="J47" s="1" t="n"/>
       <c r="K47" s="1" t="n"/>
@@ -3804,10 +3886,10 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>Matty7_</t>
-        </is>
-      </c>
-      <c r="B48" s="18" t="inlineStr">
+          <t>Alaa</t>
+        </is>
+      </c>
+      <c r="B48" s="17" t="inlineStr">
         <is>
           <t>19/12/2025</t>
         </is>
@@ -3821,11 +3903,13 @@
         <v/>
       </c>
       <c r="E48" s="5" t="n">
-        <v>34720</v>
+        <v>25100</v>
       </c>
       <c r="F48" s="1" t="n"/>
       <c r="G48" s="1" t="n"/>
-      <c r="H48" s="1" t="n"/>
+      <c r="H48" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I48" s="1" t="n"/>
       <c r="J48" s="1" t="n"/>
       <c r="K48" s="1" t="n"/>
@@ -3845,12 +3929,12 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>Alaa</t>
-        </is>
-      </c>
-      <c r="B49" s="18" t="inlineStr">
-        <is>
-          <t>19/12/2025</t>
+          <t>GiornoBrando</t>
+        </is>
+      </c>
+      <c r="B49" s="17" t="inlineStr">
+        <is>
+          <t>21/12/2025</t>
         </is>
       </c>
       <c r="C49" s="2">
@@ -3862,11 +3946,13 @@
         <v/>
       </c>
       <c r="E49" s="5" t="n">
-        <v>25100</v>
+        <v>111650</v>
       </c>
       <c r="F49" s="1" t="n"/>
       <c r="G49" s="1" t="n"/>
-      <c r="H49" s="1" t="n"/>
+      <c r="H49" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I49" s="1" t="n"/>
       <c r="J49" s="1" t="n"/>
       <c r="K49" s="1" t="n"/>
@@ -3883,48 +3969,7 @@
       <c r="V49" s="1" t="n"/>
       <c r="W49" s="1" t="n"/>
     </row>
-    <row r="50">
-      <c r="A50" s="3" t="inlineStr">
-        <is>
-          <t>GiornoBrando</t>
-        </is>
-      </c>
-      <c r="B50" s="18" t="inlineStr">
-        <is>
-          <t>21/12/2025</t>
-        </is>
-      </c>
-      <c r="C50" s="2">
-        <f>AVERAGE(F50:AB50)</f>
-        <v/>
-      </c>
-      <c r="D50" s="3">
-        <f>SUM(F50:AB50)</f>
-        <v/>
-      </c>
-      <c r="E50" s="5" t="n">
-        <v>111650</v>
-      </c>
-      <c r="F50" s="1" t="n"/>
-      <c r="G50" s="1" t="n"/>
-      <c r="H50" s="1" t="n"/>
-      <c r="I50" s="1" t="n"/>
-      <c r="J50" s="1" t="n"/>
-      <c r="K50" s="1" t="n"/>
-      <c r="L50" s="1" t="n"/>
-      <c r="M50" s="1" t="n"/>
-      <c r="N50" s="1" t="n"/>
-      <c r="O50" s="1" t="n"/>
-      <c r="P50" s="1" t="n"/>
-      <c r="Q50" s="1" t="n"/>
-      <c r="R50" s="1" t="n"/>
-      <c r="S50" s="1" t="n"/>
-      <c r="T50" s="1" t="n"/>
-      <c r="U50" s="1" t="n"/>
-      <c r="V50" s="1" t="n"/>
-      <c r="W50" s="1" t="n"/>
-    </row>
-    <row r="51" ht="15.75" customHeight="1" s="17"/>
+    <row r="51" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>
@@ -3940,7 +3985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK50"/>
+  <dimension ref="A1:AK49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -3956,10 +4001,11 @@
     <col width="10.85546875" customWidth="1" style="11" min="7" max="7"/>
     <col width="11.5703125" customWidth="1" style="11" min="8" max="14"/>
     <col width="12.5703125" customWidth="1" style="11" min="15" max="37"/>
-    <col width="9.140625" customWidth="1" style="11" min="38" max="16384"/>
+    <col width="9.140625" customWidth="1" style="11" min="38" max="38"/>
+    <col width="9.140625" customWidth="1" style="11" min="39" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="17" thickBot="1">
+    <row r="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="8" t="inlineStr">
         <is>
           <t>NOME</t>
@@ -4605,7 +4651,7 @@
     <row r="21">
       <c r="A21" s="7" t="inlineStr">
         <is>
-          <t>hh</t>
+          <t>EdoDodo</t>
         </is>
       </c>
       <c r="B21" s="12" t="inlineStr">
@@ -4614,20 +4660,20 @@
         </is>
       </c>
       <c r="C21" s="13">
-        <f>AVERAGE(D21:AL21)</f>
+        <f>AVERAGE(D22:AL22)</f>
         <v/>
       </c>
       <c r="G21" s="11" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H21" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="inlineStr">
         <is>
-          <t>EdoDodo</t>
+          <t>Luigi</t>
         </is>
       </c>
       <c r="B22" s="12" t="inlineStr">
@@ -4636,7 +4682,7 @@
         </is>
       </c>
       <c r="C22" s="13">
-        <f>AVERAGE(D22:AL22)</f>
+        <f>AVERAGE(D23:AL23)</f>
         <v/>
       </c>
       <c r="G22" s="11" t="n">
@@ -4649,7 +4695,7 @@
     <row r="23">
       <c r="A23" s="7" t="inlineStr">
         <is>
-          <t>Luigi</t>
+          <t>piegian99</t>
         </is>
       </c>
       <c r="B23" s="12" t="inlineStr">
@@ -4658,11 +4704,11 @@
         </is>
       </c>
       <c r="C23" s="13">
-        <f>AVERAGE(D23:AL23)</f>
+        <f>AVERAGE(D24:AL24)</f>
         <v/>
       </c>
       <c r="G23" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H23" s="11" t="n">
         <v>6</v>
@@ -4671,7 +4717,7 @@
     <row r="24">
       <c r="A24" s="7" t="inlineStr">
         <is>
-          <t>piegian99</t>
+          <t>tustrunz</t>
         </is>
       </c>
       <c r="B24" s="12" t="inlineStr">
@@ -4680,33 +4726,37 @@
         </is>
       </c>
       <c r="C24" s="13">
-        <f>AVERAGE(D24:AL24)</f>
+        <f>AVERAGE(D25:AL25)</f>
         <v/>
       </c>
       <c r="G24" s="11" t="n">
         <v>6</v>
       </c>
       <c r="H24" s="11" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
         <is>
-          <t>tustrunz</t>
-        </is>
-      </c>
-      <c r="B25" s="12" t="inlineStr">
-        <is>
-          <t>12/15/25</t>
-        </is>
+          <t>CARFI</t>
+        </is>
+      </c>
+      <c r="B25" s="12" t="n">
+        <v>46006</v>
       </c>
       <c r="C25" s="13">
-        <f>AVERAGE(D25:AL25)</f>
-        <v/>
+        <f>AVERAGE(D26:AL26)</f>
+        <v/>
+      </c>
+      <c r="E25" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="F25" s="11" t="n">
+        <v>6</v>
       </c>
       <c r="G25" s="11" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H25" s="11" t="n">
         <v>0</v>
@@ -4715,24 +4765,24 @@
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
         <is>
-          <t>CARFI</t>
+          <t>kakko garau</t>
         </is>
       </c>
       <c r="B26" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C26" s="13">
-        <f>AVERAGE(D26:AL26)</f>
+        <f>AVERAGE(D27:AL27)</f>
         <v/>
       </c>
       <c r="E26" s="11" t="n">
         <v>6</v>
       </c>
       <c r="F26" s="11" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G26" s="11" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H26" s="11" t="n">
         <v>0</v>
@@ -4741,24 +4791,27 @@
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
         <is>
-          <t>kakko garau</t>
+          <t>HikariNoRob</t>
         </is>
       </c>
       <c r="B27" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C27" s="13">
-        <f>AVERAGE(D27:AL27)</f>
-        <v/>
+        <f>AVERAGE(D28:AL28)</f>
+        <v/>
+      </c>
+      <c r="D27" s="11" t="n">
+        <v>6</v>
       </c>
       <c r="E27" s="11" t="n">
         <v>6</v>
       </c>
       <c r="F27" s="11" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G27" s="11" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H27" s="11" t="n">
         <v>0</v>
@@ -4767,79 +4820,76 @@
     <row r="28">
       <c r="A28" s="7" t="inlineStr">
         <is>
-          <t>HikariNoRob</t>
+          <t>D 011</t>
         </is>
       </c>
       <c r="B28" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C28" s="13">
-        <f>AVERAGE(D28:AL28)</f>
+        <f>AVERAGE(D29:AL29)</f>
         <v/>
       </c>
       <c r="D28" s="11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28" s="11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F28" s="11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G28" s="11" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="7" t="inlineStr">
         <is>
-          <t>D 011</t>
+          <t>Brazo</t>
         </is>
       </c>
       <c r="B29" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C29" s="13">
-        <f>AVERAGE(D29:AL29)</f>
+        <f>AVERAGE(D30:AL30)</f>
         <v/>
       </c>
       <c r="D29" s="11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E29" s="11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F29" s="11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G29" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H29" s="11" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="7" t="inlineStr">
         <is>
-          <t>Brazo</t>
+          <t>zombra</t>
         </is>
       </c>
       <c r="B30" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C30" s="13">
-        <f>AVERAGE(D30:AL30)</f>
-        <v/>
-      </c>
-      <c r="D30" s="11" t="n">
-        <v>6</v>
+        <f>AVERAGE(D31:AL31)</f>
+        <v/>
       </c>
       <c r="E30" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F30" s="11" t="n">
         <v>6</v>
@@ -4848,21 +4898,24 @@
         <v>6</v>
       </c>
       <c r="H30" s="11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="7" t="inlineStr">
         <is>
-          <t>zombra</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="B31" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C31" s="13">
-        <f>AVERAGE(D31:AL31)</f>
-        <v/>
+        <f>AVERAGE(D32:AL32)</f>
+        <v/>
+      </c>
+      <c r="D31" s="11" t="n">
+        <v>0</v>
       </c>
       <c r="E31" s="11" t="n">
         <v>6</v>
@@ -4874,24 +4927,24 @@
         <v>6</v>
       </c>
       <c r="H31" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="7" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>buff x-bow</t>
         </is>
       </c>
       <c r="B32" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C32" s="13">
-        <f>AVERAGE(D32:AL32)</f>
+        <f>AVERAGE(D33:AL33)</f>
         <v/>
       </c>
       <c r="D32" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E32" s="11" t="n">
         <v>6</v>
@@ -4903,20 +4956,20 @@
         <v>6</v>
       </c>
       <c r="H32" s="11" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
         <is>
-          <t>buff x-bow</t>
+          <t>Chabby</t>
         </is>
       </c>
       <c r="B33" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C33" s="13">
-        <f>AVERAGE(D33:AL33)</f>
+        <f>AVERAGE(D34:AL34)</f>
         <v/>
       </c>
       <c r="D33" s="11" t="n">
@@ -4938,14 +4991,14 @@
     <row r="34">
       <c r="A34" s="7" t="inlineStr">
         <is>
-          <t>Chabby</t>
+          <t>haha</t>
         </is>
       </c>
       <c r="B34" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C34" s="13">
-        <f>AVERAGE(D34:AL34)</f>
+        <f>AVERAGE(D35:AL35)</f>
         <v/>
       </c>
       <c r="D34" s="11" t="n">
@@ -4961,55 +5014,55 @@
         <v>6</v>
       </c>
       <c r="H34" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="7" t="inlineStr">
         <is>
-          <t>haha</t>
-        </is>
-      </c>
-      <c r="B35" s="12" t="n">
-        <v>46006</v>
+          <t>ER DANDI 1927</t>
+        </is>
+      </c>
+      <c r="B35" s="12" t="inlineStr">
+        <is>
+          <t>12/15/25</t>
+        </is>
       </c>
       <c r="C35" s="13">
-        <f>AVERAGE(D35:AL35)</f>
-        <v/>
-      </c>
-      <c r="D35" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="E35" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="F35" s="11" t="n">
-        <v>6</v>
+        <f>AVERAGE(D36:AL36)</f>
+        <v/>
       </c>
       <c r="G35" s="11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H35" s="11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="7" t="inlineStr">
         <is>
-          <t>ER DANDI 1927</t>
-        </is>
-      </c>
-      <c r="B36" s="12" t="inlineStr">
-        <is>
-          <t>12/15/25</t>
-        </is>
+          <t>Roberta</t>
+        </is>
+      </c>
+      <c r="B36" s="12" t="n">
+        <v>46006</v>
       </c>
       <c r="C36" s="13">
-        <f>AVERAGE(D36:AL36)</f>
-        <v/>
+        <f>AVERAGE(D37:AL37)</f>
+        <v/>
+      </c>
+      <c r="D36" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E36" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="F36" s="11" t="n">
+        <v>6</v>
       </c>
       <c r="G36" s="11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H36" s="11" t="n">
         <v>5</v>
@@ -5018,43 +5071,43 @@
     <row r="37">
       <c r="A37" s="7" t="inlineStr">
         <is>
-          <t>Roberta</t>
+          <t>Floky23</t>
         </is>
       </c>
       <c r="B37" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C37" s="13">
-        <f>AVERAGE(D37:AL37)</f>
+        <f>AVERAGE(D38:AL38)</f>
         <v/>
       </c>
       <c r="D37" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E37" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="F37" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G37" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="E37" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="F37" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="G37" s="11" t="n">
-        <v>6</v>
-      </c>
       <c r="H37" s="11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="7" t="inlineStr">
         <is>
-          <t>Floky23</t>
+          <t>ajejebrazorf</t>
         </is>
       </c>
       <c r="B38" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C38" s="13">
-        <f>AVERAGE(D38:AL38)</f>
+        <f>AVERAGE(D39:AL39)</f>
         <v/>
       </c>
       <c r="D38" s="11" t="n">
@@ -5067,7 +5120,7 @@
         <v>6</v>
       </c>
       <c r="G38" s="11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H38" s="11" t="n">
         <v>6</v>
@@ -5076,24 +5129,17 @@
     <row r="39">
       <c r="A39" s="7" t="inlineStr">
         <is>
-          <t>ajejebrazorf</t>
-        </is>
-      </c>
-      <c r="B39" s="12" t="n">
-        <v>46006</v>
+          <t>dado</t>
+        </is>
+      </c>
+      <c r="B39" s="12" t="inlineStr">
+        <is>
+          <t>12/15/25</t>
+        </is>
       </c>
       <c r="C39" s="13">
-        <f>AVERAGE(D39:AL39)</f>
-        <v/>
-      </c>
-      <c r="D39" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="E39" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="F39" s="11" t="n">
-        <v>6</v>
+        <f>AVERAGE(D40:AL40)</f>
+        <v/>
       </c>
       <c r="G39" s="11" t="n">
         <v>6</v>
@@ -5105,17 +5151,24 @@
     <row r="40">
       <c r="A40" s="7" t="inlineStr">
         <is>
-          <t>dado</t>
-        </is>
-      </c>
-      <c r="B40" s="12" t="inlineStr">
-        <is>
-          <t>12/15/25</t>
-        </is>
+          <t>gionny</t>
+        </is>
+      </c>
+      <c r="B40" s="12" t="n">
+        <v>46006</v>
       </c>
       <c r="C40" s="13">
-        <f>AVERAGE(D40:AL40)</f>
-        <v/>
+        <f>AVERAGE(D41:AL41)</f>
+        <v/>
+      </c>
+      <c r="D40" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E40" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="F40" s="11" t="n">
+        <v>6</v>
       </c>
       <c r="G40" s="11" t="n">
         <v>6</v>
@@ -5127,14 +5180,14 @@
     <row r="41">
       <c r="A41" s="7" t="inlineStr">
         <is>
-          <t>gionny</t>
+          <t>giosan</t>
         </is>
       </c>
       <c r="B41" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C41" s="13">
-        <f>AVERAGE(D41:AL41)</f>
+        <f>AVERAGE(D42:AL42)</f>
         <v/>
       </c>
       <c r="D41" s="11" t="n">
@@ -5156,14 +5209,14 @@
     <row r="42">
       <c r="A42" s="7" t="inlineStr">
         <is>
-          <t>giosan</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="B42" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C42" s="13">
-        <f>AVERAGE(D42:AL42)</f>
+        <f>AVERAGE(D43:AL43)</f>
         <v/>
       </c>
       <c r="D42" s="11" t="n">
@@ -5185,14 +5238,14 @@
     <row r="43">
       <c r="A43" s="7" t="inlineStr">
         <is>
-          <t>leo</t>
+          <t>RobbyCV</t>
         </is>
       </c>
       <c r="B43" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C43" s="13">
-        <f>AVERAGE(D43:AL43)</f>
+        <f>AVERAGE(D44:AL44)</f>
         <v/>
       </c>
       <c r="D43" s="11" t="n">
@@ -5214,14 +5267,14 @@
     <row r="44">
       <c r="A44" s="7" t="inlineStr">
         <is>
-          <t>RobbyCV</t>
+          <t>serra008</t>
         </is>
       </c>
       <c r="B44" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C44" s="13">
-        <f>AVERAGE(D44:AL44)</f>
+        <f>AVERAGE(D45:AL45)</f>
         <v/>
       </c>
       <c r="D44" s="11" t="n">
@@ -5243,14 +5296,14 @@
     <row r="45">
       <c r="A45" s="7" t="inlineStr">
         <is>
-          <t>serra008</t>
+          <t>sidcu js</t>
         </is>
       </c>
       <c r="B45" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C45" s="13">
-        <f>AVERAGE(D45:AL45)</f>
+        <f>AVERAGE(D46:AL46)</f>
         <v/>
       </c>
       <c r="D45" s="11" t="n">
@@ -5272,14 +5325,14 @@
     <row r="46">
       <c r="A46" s="7" t="inlineStr">
         <is>
-          <t>sidcu js</t>
+          <t>Stentaaa</t>
         </is>
       </c>
       <c r="B46" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C46" s="13">
-        <f>AVERAGE(D46:AL46)</f>
+        <f>AVERAGE(D47:AL47)</f>
         <v/>
       </c>
       <c r="D46" s="11" t="n">
@@ -5301,14 +5354,14 @@
     <row r="47">
       <c r="A47" s="7" t="inlineStr">
         <is>
-          <t>Stentaaa</t>
+          <t>th4nos</t>
         </is>
       </c>
       <c r="B47" s="12" t="n">
         <v>46006</v>
       </c>
       <c r="C47" s="13">
-        <f>AVERAGE(D47:AL47)</f>
+        <f>AVERAGE(D48:AL48)</f>
         <v/>
       </c>
       <c r="D47" s="11" t="n">
@@ -5330,24 +5383,17 @@
     <row r="48">
       <c r="A48" s="7" t="inlineStr">
         <is>
-          <t>th4nos</t>
-        </is>
-      </c>
-      <c r="B48" s="12" t="n">
-        <v>46006</v>
+          <t>xbladze</t>
+        </is>
+      </c>
+      <c r="B48" s="12" t="inlineStr">
+        <is>
+          <t>12/15/25</t>
+        </is>
       </c>
       <c r="C48" s="13">
-        <f>AVERAGE(D48:AL48)</f>
-        <v/>
-      </c>
-      <c r="D48" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="E48" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="F48" s="11" t="n">
-        <v>6</v>
+        <f>AVERAGE(D49:AL49)</f>
+        <v/>
       </c>
       <c r="G48" s="11" t="n">
         <v>6</v>
@@ -5359,42 +5405,19 @@
     <row r="49">
       <c r="A49" s="7" t="inlineStr">
         <is>
-          <t>xbladze</t>
+          <t>GiornoBrando</t>
         </is>
       </c>
       <c r="B49" s="12" t="inlineStr">
         <is>
-          <t>12/15/25</t>
+          <t>21/12/2025</t>
         </is>
       </c>
       <c r="C49" s="13">
-        <f>AVERAGE(D49:AL49)</f>
-        <v/>
-      </c>
-      <c r="G49" s="11" t="n">
-        <v>6</v>
+        <f>AVERAGE(D50:AL50)</f>
+        <v/>
       </c>
       <c r="H49" s="11" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="7" t="inlineStr">
-        <is>
-          <t>GiornoBrando</t>
-        </is>
-      </c>
-      <c r="B50" s="12" t="inlineStr">
-        <is>
-          <t>21/12/2025</t>
-        </is>
-      </c>
-      <c r="C50" s="13">
-        <f>AVERAGE(D50:AL50)</f>
-        <v/>
-      </c>
-      <c r="G50" s="11" t="n"/>
-      <c r="H50" s="11" t="n">
         <v>6</v>
       </c>
     </row>
@@ -5421,13 +5444,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14.28515625" customWidth="1" style="17" min="1" max="1"/>
-    <col width="11.5703125" customWidth="1" style="17" min="2" max="10"/>
-    <col width="12.5703125" customWidth="1" style="17" min="11" max="19"/>
+    <col width="14.28515625" customWidth="1" min="1" max="1"/>
+    <col width="11.5703125" customWidth="1" min="2" max="10"/>
+    <col width="12.5703125" customWidth="1" min="11" max="19"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="17" thickBot="1">
-      <c r="A1" s="19" t="inlineStr">
+    <row r="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>NOMEE</t>
         </is>

</xml_diff>

<commit_message>
Update Clan Games data - 2025-12-22
</commit_message>
<xml_diff>
--- a/prova.xlsx
+++ b/prova.xlsx
@@ -1837,7 +1837,7 @@
         </is>
       </c>
       <c r="C2" s="2">
-        <f>AVERAGE(F2:AB2)</f>
+        <f>ROUND(AVERAGE(F2:AB2), 0)</f>
         <v/>
       </c>
       <c r="D2" s="3">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="C3" s="2">
-        <f>AVERAGE(F3:AB3)</f>
+        <f>ROUND(AVERAGE(F3:AB3), 0)</f>
         <v/>
       </c>
       <c r="D3" s="3">
@@ -1927,7 +1927,7 @@
         </is>
       </c>
       <c r="C4" s="2">
-        <f>AVERAGE(F4:AB4)</f>
+        <f>ROUND(AVERAGE(F4:AB4), 0)</f>
         <v/>
       </c>
       <c r="D4" s="3">
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="C5" s="2">
-        <f>AVERAGE(F5:AB5)</f>
+        <f>ROUND(AVERAGE(F5:AB5), 0)</f>
         <v/>
       </c>
       <c r="D5" s="3">
@@ -2017,7 +2017,7 @@
         </is>
       </c>
       <c r="C6" s="2">
-        <f>AVERAGE(F6:AB6)</f>
+        <f>ROUND(AVERAGE(F6:AB6), 0)</f>
         <v/>
       </c>
       <c r="D6" s="3">
@@ -2032,7 +2032,7 @@
         <v>250</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="I6" s="1" t="n"/>
       <c r="J6" s="1" t="n"/>
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="C7" s="2">
-        <f>AVERAGE(F7:AB7)</f>
+        <f>ROUND(AVERAGE(F7:AB7), 0)</f>
         <v/>
       </c>
       <c r="D7" s="3">
@@ -2107,7 +2107,7 @@
         </is>
       </c>
       <c r="C8" s="2">
-        <f>AVERAGE(F8:AB8)</f>
+        <f>ROUND(AVERAGE(F8:AB8), 0)</f>
         <v/>
       </c>
       <c r="D8" s="3">
@@ -2154,7 +2154,7 @@
         </is>
       </c>
       <c r="C9" s="2">
-        <f>ROUND(AVERAGE(F9:AB9),1)</f>
+        <f>ROUND(AVERAGE(F9:AB9), 0)</f>
         <v/>
       </c>
       <c r="D9" s="3">
@@ -2201,7 +2201,7 @@
         </is>
       </c>
       <c r="C10" s="2">
-        <f>AVERAGE(F10:AB10)</f>
+        <f>ROUND(AVERAGE(F10:AB10), 0)</f>
         <v/>
       </c>
       <c r="D10" s="3">
@@ -2248,7 +2248,7 @@
         </is>
       </c>
       <c r="C11" s="2">
-        <f>AVERAGE(F11:AB11)</f>
+        <f>ROUND(AVERAGE(F11:AB11), 0)</f>
         <v/>
       </c>
       <c r="D11" s="3">
@@ -2265,7 +2265,7 @@
         <v>2100</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="I11" s="1" t="n"/>
       <c r="J11" s="1" t="n"/>
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="C12" s="2">
-        <f>AVERAGE(F12:AB12)</f>
+        <f>ROUND(AVERAGE(F12:AB12), 0)</f>
         <v/>
       </c>
       <c r="D12" s="3">
@@ -2310,7 +2310,7 @@
         <v>4000</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>3250</v>
+        <v>6650</v>
       </c>
       <c r="I12" s="1" t="n"/>
       <c r="J12" s="1" t="n"/>
@@ -2340,7 +2340,7 @@
         </is>
       </c>
       <c r="C13" s="2">
-        <f>AVERAGE(F13:AB13)</f>
+        <f>ROUND(AVERAGE(F13:AB13), 0)</f>
         <v/>
       </c>
       <c r="D13" s="3">
@@ -2385,7 +2385,7 @@
         </is>
       </c>
       <c r="C14" s="2">
-        <f>AVERAGE(F14:AB14)</f>
+        <f>ROUND(AVERAGE(F14:AB14), 0)</f>
         <v/>
       </c>
       <c r="D14" s="3">
@@ -2430,7 +2430,7 @@
         </is>
       </c>
       <c r="C15" s="2">
-        <f>AVERAGE(F15:AB15)</f>
+        <f>ROUND(AVERAGE(F15:AB15), 0)</f>
         <v/>
       </c>
       <c r="D15" s="3">
@@ -2445,7 +2445,7 @@
         <v>4000</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>5050</v>
+        <v>10100</v>
       </c>
       <c r="I15" s="1" t="n"/>
       <c r="J15" s="1" t="n"/>
@@ -2475,7 +2475,7 @@
         </is>
       </c>
       <c r="C16" s="2">
-        <f>AVERAGE(F16:AB16)</f>
+        <f>ROUND(AVERAGE(F16:AB16), 0)</f>
         <v/>
       </c>
       <c r="D16" s="3">
@@ -2520,7 +2520,7 @@
         </is>
       </c>
       <c r="C17" s="2">
-        <f>AVERAGE(F17:AB17)</f>
+        <f>ROUND(AVERAGE(F17:AB17), 0)</f>
         <v/>
       </c>
       <c r="D17" s="3">
@@ -2565,7 +2565,7 @@
         </is>
       </c>
       <c r="C18" s="2">
-        <f>AVERAGE(F18:AB18)</f>
+        <f>ROUND(AVERAGE(F18:AB18), 0)</f>
         <v/>
       </c>
       <c r="D18" s="3">
@@ -2610,7 +2610,7 @@
         </is>
       </c>
       <c r="C19" s="2">
-        <f>AVERAGE(F19:AB19)</f>
+        <f>ROUND(AVERAGE(F19:AB19), 0)</f>
         <v/>
       </c>
       <c r="D19" s="3">
@@ -2625,7 +2625,7 @@
         <v>4000</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>400</v>
+        <v>4450</v>
       </c>
       <c r="I19" s="1" t="n"/>
       <c r="J19" s="1" t="n"/>
@@ -2655,7 +2655,7 @@
         </is>
       </c>
       <c r="C20" s="2">
-        <f>AVERAGE(F20:AB20)</f>
+        <f>ROUND(AVERAGE(F20:AB20), 0)</f>
         <v/>
       </c>
       <c r="D20" s="3">
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="C21" s="2">
-        <f>AVERAGE(F21:AB21)</f>
+        <f>ROUND(AVERAGE(F21:AB21), 0)</f>
         <v/>
       </c>
       <c r="D21" s="3">
@@ -2749,7 +2749,7 @@
         </is>
       </c>
       <c r="C22" s="2">
-        <f>AVERAGE(F22:AB22)</f>
+        <f>ROUND(AVERAGE(F22:AB22), 0)</f>
         <v/>
       </c>
       <c r="D22" s="3">
@@ -2796,7 +2796,7 @@
         </is>
       </c>
       <c r="C23" s="2">
-        <f>AVERAGE(F23:AB23)</f>
+        <f>ROUND(AVERAGE(F23:AB23), 0)</f>
         <v/>
       </c>
       <c r="D23" s="3">
@@ -2843,7 +2843,7 @@
         </is>
       </c>
       <c r="C24" s="2">
-        <f>AVERAGE(F24:AB24)</f>
+        <f>ROUND(AVERAGE(F24:AB24), 0)</f>
         <v/>
       </c>
       <c r="D24" s="3">
@@ -2860,7 +2860,7 @@
         <v>4000</v>
       </c>
       <c r="H24" s="1" t="n">
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="I24" s="1" t="n"/>
       <c r="J24" s="1" t="n"/>
@@ -2890,7 +2890,7 @@
         </is>
       </c>
       <c r="C25" s="2">
-        <f>AVERAGE(F25:AB25)</f>
+        <f>ROUND(AVERAGE(F25:AB25), 0)</f>
         <v/>
       </c>
       <c r="D25" s="3">
@@ -2937,7 +2937,7 @@
         </is>
       </c>
       <c r="C26" s="2">
-        <f>AVERAGE(F26:AB26)</f>
+        <f>ROUND(AVERAGE(F26:AB26), 0)</f>
         <v/>
       </c>
       <c r="D26" s="3">
@@ -2954,7 +2954,7 @@
         <v>4000</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>2100</v>
+        <v>4200</v>
       </c>
       <c r="I26" s="1" t="n"/>
       <c r="J26" s="1" t="n"/>
@@ -2984,7 +2984,7 @@
         </is>
       </c>
       <c r="C27" s="2">
-        <f>AVERAGE(F27:AB27)</f>
+        <f>ROUND(AVERAGE(F27:AB27), 0)</f>
         <v/>
       </c>
       <c r="D27" s="3">
@@ -3031,7 +3031,7 @@
         </is>
       </c>
       <c r="C28" s="2">
-        <f>AVERAGE(F28:AB28)</f>
+        <f>ROUND(AVERAGE(F28:AB28), 0)</f>
         <v/>
       </c>
       <c r="D28" s="3">
@@ -3048,7 +3048,7 @@
         <v>4000</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>950</v>
+        <v>1900</v>
       </c>
       <c r="I28" s="1" t="n"/>
       <c r="J28" s="1" t="n"/>
@@ -3078,7 +3078,7 @@
         </is>
       </c>
       <c r="C29" s="2">
-        <f>AVERAGE(F29:AB29)</f>
+        <f>ROUND(AVERAGE(F29:AB29), 0)</f>
         <v/>
       </c>
       <c r="D29" s="3">
@@ -3121,7 +3121,7 @@
         </is>
       </c>
       <c r="C30" s="2">
-        <f>AVERAGE(F30:AB30)</f>
+        <f>ROUND(AVERAGE(F30:AB30), 0)</f>
         <v/>
       </c>
       <c r="D30" s="3">
@@ -3164,7 +3164,7 @@
         </is>
       </c>
       <c r="C31" s="2">
-        <f>AVERAGE(F31:AB31)</f>
+        <f>ROUND(AVERAGE(F31:AB31), 0)</f>
         <v/>
       </c>
       <c r="D31" s="3">
@@ -3177,7 +3177,7 @@
       <c r="F31" s="1" t="n"/>
       <c r="G31" s="1" t="n"/>
       <c r="H31" s="1" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="I31" s="1" t="n"/>
       <c r="J31" s="1" t="n"/>
@@ -3207,7 +3207,7 @@
         </is>
       </c>
       <c r="C32" s="2">
-        <f>AVERAGE(F32:AB32)</f>
+        <f>ROUND(AVERAGE(F32:AB32), 0)</f>
         <v/>
       </c>
       <c r="D32" s="3">
@@ -3250,7 +3250,7 @@
         </is>
       </c>
       <c r="C33" s="2">
-        <f>AVERAGE(F33:AB33)</f>
+        <f>ROUND(AVERAGE(F33:AB33), 0)</f>
         <v/>
       </c>
       <c r="D33" s="3">
@@ -3293,7 +3293,7 @@
         </is>
       </c>
       <c r="C34" s="2">
-        <f>AVERAGE(F34:AB34)</f>
+        <f>ROUND(AVERAGE(F34:AB34), 0)</f>
         <v/>
       </c>
       <c r="D34" s="3">
@@ -3306,7 +3306,7 @@
       <c r="F34" s="1" t="n"/>
       <c r="G34" s="1" t="n"/>
       <c r="H34" s="1" t="n">
-        <v>3850</v>
+        <v>10000</v>
       </c>
       <c r="I34" s="1" t="n"/>
       <c r="J34" s="1" t="n"/>
@@ -3336,7 +3336,7 @@
         </is>
       </c>
       <c r="C35" s="2">
-        <f>AVERAGE(F35:AB35)</f>
+        <f>ROUND(AVERAGE(F35:AB35), 0)</f>
         <v/>
       </c>
       <c r="D35" s="3">
@@ -3379,7 +3379,7 @@
         </is>
       </c>
       <c r="C36" s="2">
-        <f>AVERAGE(F36:AB36)</f>
+        <f>ROUND(AVERAGE(F36:AB36), 0)</f>
         <v/>
       </c>
       <c r="D36" s="3">
@@ -3422,7 +3422,7 @@
         </is>
       </c>
       <c r="C37" s="2">
-        <f>AVERAGE(F37:AB37)</f>
+        <f>ROUND(AVERAGE(F37:AB37), 0)</f>
         <v/>
       </c>
       <c r="D37" s="3">
@@ -3465,7 +3465,7 @@
         </is>
       </c>
       <c r="C38" s="2">
-        <f>AVERAGE(F38:AB38)</f>
+        <f>ROUND(AVERAGE(F38:AB38), 0)</f>
         <v/>
       </c>
       <c r="D38" s="3">
@@ -3478,7 +3478,7 @@
       <c r="F38" s="1" t="n"/>
       <c r="G38" s="1" t="n"/>
       <c r="H38" s="1" t="n">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="I38" s="1" t="n"/>
       <c r="J38" s="1" t="n"/>
@@ -3508,7 +3508,7 @@
         </is>
       </c>
       <c r="C39" s="2">
-        <f>AVERAGE(F39:AB39)</f>
+        <f>ROUND(AVERAGE(F39:AB39), 0)</f>
         <v/>
       </c>
       <c r="D39" s="3">
@@ -3521,7 +3521,7 @@
       <c r="F39" s="1" t="n"/>
       <c r="G39" s="1" t="n"/>
       <c r="H39" s="1" t="n">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="I39" s="1" t="n"/>
       <c r="J39" s="1" t="n"/>
@@ -3551,7 +3551,7 @@
         </is>
       </c>
       <c r="C40" s="2">
-        <f>AVERAGE(F40:AB40)</f>
+        <f>ROUND(AVERAGE(F40:AB40), 0)</f>
         <v/>
       </c>
       <c r="D40" s="3">
@@ -3594,7 +3594,7 @@
         </is>
       </c>
       <c r="C41" s="2">
-        <f>AVERAGE(F41:AB41)</f>
+        <f>ROUND(AVERAGE(F41:AB41), 0)</f>
         <v/>
       </c>
       <c r="D41" s="3">
@@ -3637,7 +3637,7 @@
         </is>
       </c>
       <c r="C42" s="2">
-        <f>AVERAGE(F42:AB42)</f>
+        <f>ROUND(AVERAGE(F42:AB42), 0)</f>
         <v/>
       </c>
       <c r="D42" s="3">
@@ -3680,7 +3680,7 @@
         </is>
       </c>
       <c r="C43" s="2">
-        <f>AVERAGE(F43:AB43)</f>
+        <f>ROUND(AVERAGE(F43:AB43), 0)</f>
         <v/>
       </c>
       <c r="D43" s="3">
@@ -3723,7 +3723,7 @@
         </is>
       </c>
       <c r="C44" s="2">
-        <f>AVERAGE(F44:AB44)</f>
+        <f>ROUND(AVERAGE(F44:AB44), 0)</f>
         <v/>
       </c>
       <c r="D44" s="3">
@@ -3766,7 +3766,7 @@
         </is>
       </c>
       <c r="C45" s="2">
-        <f>AVERAGE(F45:AB45)</f>
+        <f>ROUND(AVERAGE(F45:AB45), 0)</f>
         <v/>
       </c>
       <c r="D45" s="3">
@@ -3809,7 +3809,7 @@
         </is>
       </c>
       <c r="C46" s="2">
-        <f>AVERAGE(F46:AB46)</f>
+        <f>ROUND(AVERAGE(F46:AB46), 0)</f>
         <v/>
       </c>
       <c r="D46" s="3">
@@ -3852,7 +3852,7 @@
         </is>
       </c>
       <c r="C47" s="2">
-        <f>AVERAGE(F47:AB47)</f>
+        <f>ROUND(AVERAGE(F47:AB47), 0)</f>
         <v/>
       </c>
       <c r="D47" s="3">
@@ -3895,7 +3895,7 @@
         </is>
       </c>
       <c r="C48" s="2">
-        <f>AVERAGE(F48:AB48)</f>
+        <f>ROUND(AVERAGE(F48:AB48), 0)</f>
         <v/>
       </c>
       <c r="D48" s="3">
@@ -3938,7 +3938,7 @@
         </is>
       </c>
       <c r="C49" s="2">
-        <f>AVERAGE(F49:AB49)</f>
+        <f>ROUND(AVERAGE(F49:AB49), 0)</f>
         <v/>
       </c>
       <c r="D49" s="3">

</xml_diff>

<commit_message>
Update Clan Games data - 2025-12-23
</commit_message>
<xml_diff>
--- a/prova.xlsx
+++ b/prova.xlsx
@@ -1886,12 +1886,12 @@
         <v/>
       </c>
       <c r="E3" s="5" t="n">
-        <v>26800</v>
+        <v>30700</v>
       </c>
       <c r="F3" s="1" t="n"/>
       <c r="G3" s="1" t="n"/>
       <c r="H3" s="1" t="n">
-        <v>6150</v>
+        <v>10050</v>
       </c>
       <c r="I3" s="1" t="n"/>
       <c r="J3" s="1" t="n"/>

</xml_diff>